<commit_message>
Unit Test, DB, TODO
Unit Test, DB, TODO
</commit_message>
<xml_diff>
--- a/Definitions/d_Definitions_unit_test.xlsx
+++ b/Definitions/d_Definitions_unit_test.xlsx
@@ -2159,7 +2159,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2170,9 +2170,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2197,15 +2194,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2231,9 +2222,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2247,6 +2235,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2607,7 +2604,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="21" t="s">
         <v>247</v>
       </c>
     </row>
@@ -2615,7 +2612,7 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="21" t="s">
         <v>248</v>
       </c>
     </row>
@@ -2623,7 +2620,7 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="21" t="s">
         <v>249</v>
       </c>
     </row>
@@ -2631,7 +2628,7 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="22" t="s">
         <v>250</v>
       </c>
     </row>
@@ -2639,15 +2636,15 @@
       <c r="A6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="22" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="22" t="s">
         <v>252</v>
       </c>
     </row>
@@ -2655,20 +2652,20 @@
       <c r="A8" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="22" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="22" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="18" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2711,131 +2708,131 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="40"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="22" customFormat="1">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:2" s="19" customFormat="1">
+      <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="22" customFormat="1">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:2" s="19" customFormat="1">
+      <c r="A5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="22" customFormat="1">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:2" s="19" customFormat="1">
+      <c r="A6" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="22" customFormat="1"/>
+    <row r="7" spans="1:2" s="19" customFormat="1"/>
     <row r="9" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="10" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="41"/>
+      <c r="B10" s="40"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="19" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="13" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="17" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="39" t="s">
         <v>228</v>
       </c>
-      <c r="B17" s="41"/>
+      <c r="B17" s="40"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="19" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="23" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="B23" s="41"/>
+      <c r="B23" s="40"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="19" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="27" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="39" t="s">
         <v>238</v>
       </c>
-      <c r="B27" s="41"/>
+      <c r="B27" s="40"/>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="39"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="35" t="s">
         <v>271</v>
       </c>
-      <c r="B31" s="37"/>
+      <c r="B31" s="36"/>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
@@ -2846,10 +2843,10 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="37"/>
+      <c r="B34" s="36"/>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
@@ -2860,22 +2857,22 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="30"/>
-      <c r="B36" s="31" t="s">
+      <c r="A36" s="26"/>
+      <c r="B36" s="27" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="30"/>
-      <c r="B37" s="31" t="s">
+      <c r="A37" s="26"/>
+      <c r="B37" s="27" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="27" t="s">
         <v>262</v>
       </c>
     </row>
@@ -2915,8 +2912,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="112.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="112.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1">
@@ -2928,342 +2925,342 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="40"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>279</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="37"/>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="41"/>
+      <c r="B5" s="40"/>
     </row>
     <row r="6" spans="1:2" ht="45">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="90">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60">
-      <c r="A9" s="43"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="42"/>
+      <c r="B9" s="9" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="75">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="240">
-      <c r="A12" s="43"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="42"/>
+      <c r="B12" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="60">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="45">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="225">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="45">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="315">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="30" t="s">
         <v>301</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="135">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="45">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="60">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="90">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="20" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="75">
-      <c r="A35" s="39"/>
-      <c r="B35" s="16" t="s">
+      <c r="A35" s="38"/>
+      <c r="B35" s="14" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="37" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A37" s="40" t="s">
+      <c r="A37" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="B37" s="41"/>
+      <c r="B37" s="40"/>
     </row>
     <row r="38" spans="1:2" ht="135">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="28" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="29" t="s">
         <v>283</v>
       </c>
-      <c r="B39" s="33" t="s">
+      <c r="B39" s="29" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="33" t="s">
+      <c r="A40" s="29" t="s">
         <v>285</v>
       </c>
-      <c r="B40" s="33" t="s">
+      <c r="B40" s="29" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="29" t="s">
         <v>286</v>
       </c>
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="29" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="33" t="s">
+      <c r="A42" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="29" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="33" t="s">
+      <c r="A43" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="B43" s="33" t="s">
+      <c r="B43" s="29" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="33" t="s">
+      <c r="A44" s="29" t="s">
         <v>293</v>
       </c>
-      <c r="B44" s="33" t="s">
+      <c r="B44" s="29" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="29" t="s">
         <v>295</v>
       </c>
-      <c r="B45" s="33" t="s">
+      <c r="B45" s="29" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="33" t="s">
+      <c r="A46" s="29" t="s">
         <v>297</v>
       </c>
-      <c r="B46" s="33" t="s">
+      <c r="B46" s="29" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="30" t="s">
         <v>299</v>
       </c>
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="30" t="s">
         <v>300</v>
       </c>
     </row>
@@ -3311,28 +3308,28 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="40"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="10" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="41"/>
+      <c r="B10" s="40"/>
     </row>
     <row r="11" spans="1:2" ht="45">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="20" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="38" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -3340,31 +3337,31 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="30">
-      <c r="A13" s="39"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="39"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="39"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="39"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="39"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="4" t="s">
         <v>35</v>
       </c>
@@ -3373,7 +3370,7 @@
       <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="20" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3381,7 +3378,7 @@
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="20" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3412,14 +3409,14 @@
   <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="113.140625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="113.140625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1">
@@ -3431,438 +3428,443 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="40"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="41"/>
+      <c r="B5" s="40"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="16" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="60">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="16" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="31" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="43"/>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="42"/>
+      <c r="B11" s="31" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="31" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="31" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="31" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="60">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="31" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="31" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="31" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="31" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="39"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="38"/>
+      <c r="B19" s="31" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="60">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="31" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="31" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="105">
-      <c r="A22" s="44"/>
-      <c r="B22" s="23" t="s">
+      <c r="A22" s="43"/>
+      <c r="B22" s="31" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30">
-      <c r="A23" s="44"/>
-      <c r="B23" s="15" t="s">
+      <c r="A23" s="43"/>
+      <c r="B23" s="31" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="31" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="31" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="31" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30">
-      <c r="A27" s="44"/>
-      <c r="B27" s="15" t="s">
+      <c r="A27" s="43"/>
+      <c r="B27" s="31" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="75">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="31" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="31" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="45">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="31" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="44"/>
-      <c r="B31" s="15" t="s">
+      <c r="A31" s="43"/>
+      <c r="B31" s="31" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="60">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="31" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="31" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="30">
-      <c r="A34" s="44"/>
-      <c r="B34" s="15" t="s">
+      <c r="A34" s="43"/>
+      <c r="B34" s="31" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="31" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="44"/>
-      <c r="B36" s="15" t="s">
+      <c r="A36" s="43"/>
+      <c r="B36" s="31" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="13" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="45">
-      <c r="A38" s="39"/>
-      <c r="B38" s="15" t="s">
+      <c r="A38" s="38"/>
+      <c r="B38" s="31" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="30">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="31" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="45">
-      <c r="A40" s="39"/>
-      <c r="B40" s="15" t="s">
+      <c r="A40" s="38"/>
+      <c r="B40" s="31" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="39"/>
-      <c r="B41" s="18" t="s">
+      <c r="A41" s="38"/>
+      <c r="B41" s="15" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="31" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="31" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="30">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="31" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="31" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="31" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="31" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="31" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="30">
-      <c r="A49" s="39" t="s">
+      <c r="A49" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="31" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="45">
-      <c r="A50" s="39"/>
-      <c r="B50" s="23" t="s">
+      <c r="A50" s="38"/>
+      <c r="B50" s="31" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="75">
-      <c r="A51" s="43" t="s">
+      <c r="A51" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="B51" s="23" t="s">
+      <c r="B51" s="31" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="90">
-      <c r="A52" s="43"/>
-      <c r="B52" s="16" t="s">
+      <c r="A52" s="42"/>
+      <c r="B52" s="31" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="45">
-      <c r="A53" s="43"/>
-      <c r="B53" s="16" t="s">
+      <c r="A53" s="42"/>
+      <c r="B53" s="31" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30">
-      <c r="A54" s="16" t="s">
+      <c r="A54" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="31" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="75">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="31" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="45">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="B56" s="31" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="120">
-      <c r="A57" s="39"/>
-      <c r="B57" s="23" t="s">
+      <c r="A57" s="38"/>
+      <c r="B57" s="31" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="30">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="B58" s="19" t="s">
+      <c r="B58" s="31" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="31" t="s">
         <v>195</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="B59" s="31" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="B60" s="19" t="s">
+      <c r="B60" s="31" t="s">
         <v>198</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A37:A38"/>
@@ -3872,11 +3874,6 @@
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="Mockito!A2" display="Up"/>
@@ -3900,7 +3897,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="60" customWidth="1"/>
-    <col min="2" max="2" width="103.7109375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="103.7109375" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3912,28 +3909,28 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="36"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="36"/>
     </row>
     <row r="9" spans="1:2" ht="60">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="16" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
-      <c r="A10" s="47"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="46"/>
+      <c r="B10" s="16" t="s">
         <v>204</v>
       </c>
     </row>
@@ -3941,7 +3938,7 @@
       <c r="A11" t="s">
         <v>205</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="16" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3949,7 +3946,7 @@
       <c r="A12" t="s">
         <v>206</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="16" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3957,79 +3954,79 @@
       <c r="A13" t="s">
         <v>208</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="16" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="75">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="47" t="s">
         <v>211</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="17" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="45">
-      <c r="A15" s="48"/>
-      <c r="B15" s="20" t="s">
+      <c r="A15" s="47"/>
+      <c r="B15" s="17" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120">
-      <c r="A16" s="48"/>
-      <c r="B16" s="20" t="s">
+      <c r="A16" s="47"/>
+      <c r="B16" s="17" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="45">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="17" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="17" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="17" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="45">
-      <c r="A20" s="47"/>
-      <c r="B20" s="20" t="s">
+      <c r="A20" s="46"/>
+      <c r="B20" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="44" t="s">
         <v>221</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="17" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="90">
-      <c r="A22" s="45"/>
-      <c r="B22" s="20" t="s">
+      <c r="A22" s="44"/>
+      <c r="B22" s="17" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="17" t="s">
         <v>226</v>
       </c>
     </row>
@@ -4075,16 +4072,16 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="36"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="36"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
@@ -4103,26 +4100,26 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="45">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="24" t="s">
         <v>259</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="23" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="60">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="24" t="s">
         <v>256</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="23" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="23" t="s">
         <v>260</v>
       </c>
     </row>
@@ -4163,24 +4160,24 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="36"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="25" t="s">
         <v>272</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="36"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
@@ -4194,7 +4191,7 @@
       <c r="A9" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>90</v>
       </c>
     </row>
@@ -4210,63 +4207,63 @@
       <c r="A11" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="75">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="48" t="s">
         <v>264</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="25" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="49"/>
-      <c r="B13" s="29" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="25" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="45">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="25" t="s">
         <v>267</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="25" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="48" t="s">
         <v>269</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="25" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="49"/>
-      <c r="B16" s="29" t="s">
+      <c r="A16" s="48"/>
+      <c r="B16" s="25" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="48" t="s">
         <v>278</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="25" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="50"/>
-      <c r="B18" s="29" t="s">
+      <c r="A18" s="49"/>
+      <c r="B18" s="25" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="50"/>
-      <c r="B19" s="29" t="s">
+      <c r="A19" s="49"/>
+      <c r="B19" s="25" t="s">
         <v>276</v>
       </c>
     </row>
@@ -4312,46 +4309,46 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="40"/>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="7" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="41"/>
+      <c r="B7" s="40"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="11" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="41"/>
+      <c r="B11" s="40"/>
     </row>
     <row r="12" spans="1:2" ht="30">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="19" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="19" t="s">
         <v>234</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Collections, Multithreading, Todo, Kafka
</commit_message>
<xml_diff>
--- a/Definitions/d_Definitions_unit_test.xlsx
+++ b/Definitions/d_Definitions_unit_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="994" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="994" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="306">
   <si>
     <t>Topics</t>
   </si>
@@ -1078,9 +1078,6 @@
 });</t>
   </si>
   <si>
-    <t>thenAnswer(..) - this is used for argument matchig means return different values based on arguments to method being mocked</t>
-  </si>
-  <si>
     <t>Mockito.verify()</t>
   </si>
   <si>
@@ -1263,9 +1260,6 @@
   <si>
     <t>1. To mock static methods in mock framework
 2. Mockito uses the proxy pattern to facilitate mocking. Powermock uses a custom class loader and byte code manipulation to add these extra capabilities. When using these two frameworks in conjunction my preference is to leverage Mockito directly as much as possible and only use power mock for your exceptional requirements.</t>
-  </si>
-  <si>
-    <t>Powermock offers the capability to create stubs for static method calls. We need to declare that we want to mock static methods for the class, then perform stubbing and verification</t>
   </si>
   <si>
     <t>Steps to have powermock</t>
@@ -1986,6 +1980,13 @@
   </si>
   <si>
     <t>Eclipse Workspace</t>
+  </si>
+  <si>
+    <t>thenAnswer(..) - this is used for argument matching means return different values based on arguments to method being mocked</t>
+  </si>
+  <si>
+    <t>Powermock offers the capability to create stubs for static method calls. 
+We need to declare that we want to mock static methods for the class, then perform stubbing and verification</t>
   </si>
 </sst>
 </file>
@@ -2180,7 +2181,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2266,6 +2267,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2608,7 +2613,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2630,7 +2635,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2638,7 +2643,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2646,7 +2651,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2654,7 +2659,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2662,7 +2667,7 @@
         <v>66</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2670,7 +2675,7 @@
         <v>80</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2678,7 +2683,7 @@
         <v>89</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2686,12 +2691,12 @@
         <v>103</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2711,11 +2716,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2733,194 +2738,104 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="42"/>
+      <c r="A2" s="43" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="44"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="19" customFormat="1">
-      <c r="A4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="19" customFormat="1">
-      <c r="A5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="19" customFormat="1">
-      <c r="A6" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="19" customFormat="1"/>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1"/>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A10" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="42"/>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="19" t="s">
+      <c r="A3" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B3" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1"/>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A17" s="41" t="s">
-        <v>224</v>
-      </c>
-      <c r="B17" s="42"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="19" t="s">
+    <row r="7" spans="1:2" ht="15.75" thickBot="1"/>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A8" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="44"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B9" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1"/>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A23" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" s="42"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1"/>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A27" s="41" t="s">
-        <v>234</v>
-      </c>
-      <c r="B27" s="42"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="40"/>
-      <c r="B29" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="37" t="s">
-        <v>267</v>
-      </c>
-      <c r="B31" s="38"/>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
+    <row r="11" spans="1:2" ht="15.75" thickBot="1"/>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A12" s="43" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12" s="44"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="39" t="s">
+        <v>265</v>
+      </c>
+      <c r="B16" s="40"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>81</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B17" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="37" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="38"/>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
+      <c r="B19" s="40"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="26"/>
-      <c r="B36" s="27" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="26"/>
+      <c r="B21" s="27" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="26"/>
-      <c r="B37" s="27" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="26"/>
+      <c r="B22" s="27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="26" t="s">
-        <v>257</v>
-      </c>
-      <c r="B38" s="27" t="s">
-        <v>258</v>
+    <row r="23" spans="1:2">
+      <c r="A23" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A28:A29"/>
+  <mergeCells count="5">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="Materials!A1" display="Up"/>
     <hyperlink ref="A1" location="Topics!A10" display="Topics"/>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B28" r:id="rId2"/>
-    <hyperlink ref="B35" r:id="rId3"/>
-    <hyperlink ref="B38" r:id="rId4"/>
-    <hyperlink ref="B36" r:id="rId5"/>
-    <hyperlink ref="B37" r:id="rId6"/>
+    <hyperlink ref="B20" r:id="rId1"/>
+    <hyperlink ref="B23" r:id="rId2"/>
+    <hyperlink ref="B21" r:id="rId3"/>
+    <hyperlink ref="B22" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2928,11 +2843,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2950,384 +2865,436 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="42"/>
+      <c r="B2" s="44"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="43" t="s">
-        <v>275</v>
-      </c>
-      <c r="B3" s="39"/>
+      <c r="A3" s="45" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" s="41"/>
     </row>
     <row r="5" spans="1:2" s="36" customFormat="1" ht="15.75" thickBot="1">
       <c r="A5" s="35"/>
       <c r="B5" s="35"/>
     </row>
     <row r="6" spans="1:2" s="36" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A6" s="41" t="s">
-        <v>303</v>
-      </c>
-      <c r="B6" s="42"/>
+      <c r="A6" s="43" t="s">
+        <v>301</v>
+      </c>
+      <c r="B6" s="44"/>
     </row>
     <row r="7" spans="1:2" s="36" customFormat="1">
       <c r="A7" s="36" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="36" customFormat="1" ht="15.75" thickBot="1">
       <c r="A8" s="35"/>
       <c r="B8" s="35"/>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A9" s="41" t="s">
+    <row r="9" spans="1:2" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A9" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" s="44"/>
+    </row>
+    <row r="10" spans="1:2" s="38" customFormat="1">
+      <c r="A10" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="38" customFormat="1">
+      <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="38" customFormat="1">
+      <c r="A12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="38" customFormat="1">
+      <c r="A13" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="38" customFormat="1">
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+    </row>
+    <row r="15" spans="1:2" s="38" customFormat="1">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+    </row>
+    <row r="16" spans="1:2" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A17" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="42"/>
-    </row>
-    <row r="10" spans="1:2" ht="45">
-      <c r="A10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="90">
-      <c r="A12" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="60">
-      <c r="A13" s="44"/>
-      <c r="B13" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="30">
-      <c r="A14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="75">
-      <c r="A15" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="240">
-      <c r="A16" s="44"/>
-      <c r="B16" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="60">
-      <c r="A17" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>56</v>
-      </c>
+      <c r="B17" s="44"/>
     </row>
     <row r="18" spans="1:2" ht="45">
       <c r="A18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="90">
+      <c r="A20" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="60">
+      <c r="A21" s="46"/>
+      <c r="B21" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="30">
+      <c r="A22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="75">
+      <c r="A23" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="240">
+      <c r="A24" s="46"/>
+      <c r="B24" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="60">
+      <c r="A25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="45">
+      <c r="A26" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="225">
-      <c r="A19" s="5" t="s">
+    <row r="27" spans="1:2" ht="225">
+      <c r="A27" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B27" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="45">
-      <c r="A20" s="5" t="s">
+    <row r="28" spans="1:2" ht="45">
+      <c r="A28" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="315">
-      <c r="A21" s="30" t="s">
+    <row r="29" spans="1:2" ht="315">
+      <c r="A29" s="30" t="s">
+        <v>295</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="135">
+      <c r="A30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="35" t="s">
         <v>297</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="135">
-      <c r="A22" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="35" t="s">
-        <v>299</v>
-      </c>
-      <c r="B24" s="35" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="30">
-      <c r="A26" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="30">
-      <c r="A27" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="30">
-      <c r="A28" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B28" s="35" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="45">
-      <c r="A29" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B29" s="35" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="60">
-      <c r="A31" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>107</v>
+      <c r="B32" s="35" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>116</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="30">
       <c r="A34" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="60">
+        <v>117</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="30">
       <c r="A35" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>113</v>
+        <v>118</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="30">
       <c r="A36" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="45">
+      <c r="A37" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="60">
+      <c r="A39" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="60">
+      <c r="A43" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="30">
+      <c r="A44" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B44" s="12" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="12" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B45" s="12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="90">
-      <c r="A38" s="40" t="s">
+    <row r="46" spans="1:2" ht="90">
+      <c r="A46" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="75">
+      <c r="A47" s="42"/>
+      <c r="B47" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="B38" s="20" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="75">
-      <c r="A39" s="40"/>
-      <c r="B39" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" thickBot="1"/>
-    <row r="41" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A41" s="41" t="s">
+    </row>
+    <row r="48" spans="1:2" ht="15.75" thickBot="1"/>
+    <row r="49" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A49" s="43" t="s">
+        <v>274</v>
+      </c>
+      <c r="B49" s="44"/>
+    </row>
+    <row r="50" spans="1:2" ht="135">
+      <c r="A50" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="B50" s="28" t="s">
         <v>276</v>
       </c>
-      <c r="B41" s="42"/>
-    </row>
-    <row r="42" spans="1:2" ht="135">
-      <c r="A42" s="28" t="s">
+    </row>
+    <row r="51" spans="1:2" ht="120">
+      <c r="A51" s="29" t="s">
         <v>277</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B51" s="29" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="120">
-      <c r="A43" s="29" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="29" t="s">
         <v>279</v>
       </c>
-      <c r="B43" s="29" t="s">
+      <c r="B52" s="29" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="29" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="29" t="s">
+      <c r="B53" s="29" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="29" t="s">
         <v>281</v>
       </c>
-      <c r="B44" s="29" t="s">
+      <c r="B54" s="29" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="B55" s="29" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="29" t="s">
-        <v>282</v>
-      </c>
-      <c r="B45" s="29" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="29" t="s">
-        <v>283</v>
-      </c>
-      <c r="B46" s="29" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="29" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="B47" s="29" t="s">
+      <c r="B56" s="29" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="29" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="29" t="s">
         <v>289</v>
       </c>
-      <c r="B48" s="29" t="s">
+      <c r="B57" s="29" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="29" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="B49" s="29" t="s">
+      <c r="B58" s="29" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="29" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="30" t="s">
         <v>293</v>
       </c>
-      <c r="B50" s="29" t="s">
+      <c r="B59" s="30" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="30" t="s">
-        <v>295</v>
-      </c>
-      <c r="B51" s="30" t="s">
-        <v>296</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="Junit!A2" display="Up"/>
     <hyperlink ref="A1" location="Topics!A2" display="Topics"/>
     <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="B13" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3337,7 +3304,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3355,17 +3322,38 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="42"/>
+      <c r="B2" s="44"/>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1"/>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A5" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="B5" s="44"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="42"/>
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="10" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="42"/>
+      <c r="B10" s="44"/>
     </row>
     <row r="11" spans="1:2" ht="45">
       <c r="A11" s="4" t="s">
@@ -3376,7 +3364,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="42" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -3384,31 +3372,31 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="30">
-      <c r="A13" s="40"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="40"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="40"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="40"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="40"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="4" t="s">
         <v>35</v>
       </c>
@@ -3418,7 +3406,7 @@
         <v>36</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30">
@@ -3426,7 +3414,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -3438,14 +3426,17 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="'Easy Mock'!A2" display="Up"/>
     <hyperlink ref="A1" location="Topics!A3" display="Topics"/>
+    <hyperlink ref="B6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3453,11 +3444,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3475,10 +3466,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="42"/>
+      <c r="B2" s="44"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="13" t="s">
@@ -3488,439 +3479,500 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1"/>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:2" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+    </row>
+    <row r="6" spans="1:2" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A6" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="B6" s="44"/>
+    </row>
+    <row r="7" spans="1:2" s="38" customFormat="1">
+      <c r="A7" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="38" customFormat="1">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="38" customFormat="1">
+      <c r="A9" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+    </row>
+    <row r="11" spans="1:2" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A11" s="43" t="s">
+        <v>301</v>
+      </c>
+      <c r="B11" s="44"/>
+    </row>
+    <row r="12" spans="1:2" s="38" customFormat="1">
+      <c r="A12" s="38" t="s">
+        <v>303</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="38" customFormat="1">
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+    </row>
+    <row r="14" spans="1:2" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A15" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="42"/>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="13" t="s">
+      <c r="B15" s="44"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B16" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="60">
+      <c r="A17" s="16" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="60">
-      <c r="A7" s="16" t="s">
+      <c r="B17" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30">
-      <c r="A8" s="13" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="30">
+      <c r="A18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B18" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30">
-      <c r="A9" s="31" t="s">
+    <row r="19" spans="1:2" ht="30">
+      <c r="A19" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B19" s="31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30">
-      <c r="A10" s="44" t="s">
+    <row r="20" spans="1:2" ht="30">
+      <c r="A20" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="46"/>
+      <c r="B21" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="90">
+      <c r="A24" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="60">
+      <c r="A25" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="30">
+      <c r="A26" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="42"/>
+      <c r="B29" s="31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="60">
+      <c r="A30" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="105">
+      <c r="A32" s="47"/>
+      <c r="B32" s="31" t="s">
         <v>235</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="44"/>
-      <c r="B11" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="90">
-      <c r="A14" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="60">
-      <c r="A15" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="30">
-      <c r="A16" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="40"/>
-      <c r="B19" s="31" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="60">
-      <c r="A20" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="31" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="B21" s="31" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="105">
-      <c r="A22" s="45"/>
-      <c r="B22" s="31" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="30">
-      <c r="A23" s="45"/>
-      <c r="B23" s="31" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="30">
+      <c r="A33" s="47"/>
+      <c r="B33" s="31" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="33" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B34" s="31" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="33" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B35" s="31" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="45" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B36" s="31" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="30">
-      <c r="A27" s="45"/>
-      <c r="B27" s="31" t="s">
+    <row r="37" spans="1:2" ht="30">
+      <c r="A37" s="47"/>
+      <c r="B37" s="31" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="75">
-      <c r="A28" s="33" t="s">
+    <row r="38" spans="1:2" ht="75">
+      <c r="A38" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B38" s="31" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="33" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B39" s="31" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="45">
-      <c r="A30" s="45" t="s">
+    <row r="40" spans="1:2" ht="45">
+      <c r="A40" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B40" s="31" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="45"/>
-      <c r="B31" s="31" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="47"/>
+      <c r="B41" s="31" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="60">
-      <c r="A32" s="33" t="s">
+    <row r="42" spans="1:2" ht="60">
+      <c r="A42" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B42" s="31" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="45" t="s">
+    <row r="43" spans="1:2">
+      <c r="A43" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="B33" s="31" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="30">
-      <c r="A34" s="45"/>
-      <c r="B34" s="31" t="s">
+      <c r="B43" s="31" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="30">
+      <c r="A44" s="47"/>
+      <c r="B44" s="31" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="45" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B45" s="31" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="45"/>
-      <c r="B36" s="31" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="47"/>
+      <c r="B46" s="31" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="40" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="42" t="s">
+        <v>304</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="45">
+      <c r="A48" s="42"/>
+      <c r="B48" s="31" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="30">
+      <c r="A49" s="42" t="s">
         <v>159</v>
       </c>
-      <c r="B37" s="13" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="45">
-      <c r="A38" s="40"/>
-      <c r="B38" s="31" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="30">
-      <c r="A39" s="40" t="s">
+      <c r="B49" s="31" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="45">
+      <c r="A50" s="42"/>
+      <c r="B50" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="B39" s="31" t="s">
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="42"/>
+      <c r="B51" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="31" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="45">
-      <c r="A40" s="40"/>
-      <c r="B40" s="31" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="40"/>
-      <c r="B41" s="15" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="31" t="s">
+      <c r="B52" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="B42" s="31" t="s">
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="31" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="31" t="s">
+      <c r="B53" s="31" t="s">
         <v>165</v>
-      </c>
-      <c r="B43" s="31" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="30">
-      <c r="A44" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="B44" s="31" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="31" t="s">
-        <v>168</v>
-      </c>
-      <c r="B45" s="31" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="B46" s="31" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="31" t="s">
-        <v>172</v>
-      </c>
-      <c r="B47" s="31" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="B48" s="31" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="30">
-      <c r="A49" s="40" t="s">
-        <v>239</v>
-      </c>
-      <c r="B49" s="31" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="45">
-      <c r="A50" s="40"/>
-      <c r="B50" s="31" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="75">
-      <c r="A51" s="44" t="s">
-        <v>177</v>
-      </c>
-      <c r="B51" s="31" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="90">
-      <c r="A52" s="44"/>
-      <c r="B52" s="31" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="45">
-      <c r="A53" s="44"/>
-      <c r="B53" s="31" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30">
       <c r="A54" s="31" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="B54" s="31" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="B55" s="31" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B56" s="31" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="B57" s="31" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="B58" s="31" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="30">
+      <c r="A59" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="B59" s="31" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="45">
+      <c r="A60" s="42"/>
+      <c r="B60" s="31" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="75">
+      <c r="A61" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="B61" s="31" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="90">
+      <c r="A62" s="46"/>
+      <c r="B62" s="31" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="45">
+      <c r="A63" s="46"/>
+      <c r="B63" s="31" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="30">
+      <c r="A64" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="B64" s="31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="75">
+      <c r="A65" s="31" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="75">
-      <c r="A55" s="31" t="s">
+      <c r="B65" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="B55" s="31" t="s">
+    </row>
+    <row r="66" spans="1:2" ht="45">
+      <c r="A66" s="42" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" ht="45">
-      <c r="A56" s="40" t="s">
+      <c r="B66" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="B56" s="31" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="120">
-      <c r="A57" s="40"/>
-      <c r="B57" s="31" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="30">
-      <c r="A58" s="31" t="s">
+    </row>
+    <row r="67" spans="1:2" ht="120">
+      <c r="A67" s="42"/>
+      <c r="B67" s="31" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="30">
+      <c r="A68" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="B68" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="B58" s="31" t="s">
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="31" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="31" t="s">
+      <c r="B69" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="B59" s="31" t="s">
+    </row>
+    <row r="70" spans="1:2" ht="30">
+      <c r="A70" s="31" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" ht="30">
-      <c r="A60" s="31" t="s">
+      <c r="B70" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="B60" s="31" t="s">
-        <v>194</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A10:A11"/>
+  <mergeCells count="16">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A20:A21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="Mockito!A2" display="Up"/>
@@ -3936,9 +3988,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3956,125 +4008,125 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="40"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="40"/>
     </row>
     <row r="9" spans="1:2" ht="60">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>199</v>
-      </c>
     </row>
     <row r="10" spans="1:2" ht="30">
-      <c r="A10" s="48"/>
-      <c r="B10" s="16" t="s">
-        <v>200</v>
+      <c r="A10" s="50"/>
+      <c r="B10" s="37" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="120">
       <c r="A11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45">
       <c r="A13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B13" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="75">
+      <c r="A14" s="51" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="75">
-      <c r="A14" s="49" t="s">
+      <c r="B14" s="17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="45">
+      <c r="A15" s="51"/>
+      <c r="B15" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="B14" s="17" t="s">
+    </row>
+    <row r="16" spans="1:2" ht="120">
+      <c r="A16" s="51"/>
+      <c r="B16" s="17" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="45">
-      <c r="A15" s="49"/>
-      <c r="B15" s="17" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="120">
-      <c r="A16" s="49"/>
-      <c r="B16" s="17" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="45">
       <c r="A17" s="19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30">
+      <c r="A19" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B19" s="17" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30">
-      <c r="A19" s="48" t="s">
+    <row r="20" spans="1:2" ht="45">
+      <c r="A20" s="50"/>
+      <c r="B20" s="17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30">
+      <c r="A21" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B21" s="17" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="45">
-      <c r="A20" s="48"/>
-      <c r="B20" s="17" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30">
-      <c r="A21" s="46" t="s">
-        <v>217</v>
-      </c>
-      <c r="B21" s="17" t="s">
+    <row r="22" spans="1:2" ht="90">
+      <c r="A22" s="48"/>
+      <c r="B22" s="17" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="90">
-      <c r="A22" s="46"/>
-      <c r="B22" s="17" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30">
       <c r="A23" s="19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -4119,16 +4171,16 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="40"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="38"/>
+      <c r="B7" s="40"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
@@ -4148,26 +4200,26 @@
     </row>
     <row r="10" spans="1:2" ht="45">
       <c r="A10" s="24" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="60">
       <c r="A11" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45">
       <c r="A12" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="23" t="s">
         <v>254</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -4207,24 +4259,24 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="40"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="25" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="38"/>
+      <c r="B7" s="40"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
@@ -4259,59 +4311,59 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="75">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="52" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="52"/>
+      <c r="B13" s="25" t="s">
         <v>260</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="50"/>
-      <c r="B13" s="25" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="45">
       <c r="A14" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30">
+      <c r="A15" s="52" t="s">
         <v>263</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B15" s="25" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="52"/>
+      <c r="B16" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="30">
-      <c r="A15" s="50" t="s">
-        <v>265</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="50"/>
-      <c r="B16" s="25" t="s">
-        <v>266</v>
-      </c>
-    </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="50" t="s">
-        <v>274</v>
+      <c r="A17" s="52" t="s">
+        <v>272</v>
       </c>
       <c r="B17" s="25" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="53"/>
+      <c r="B18" s="25" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="53"/>
+      <c r="B19" s="25" t="s">
         <v>270</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="51"/>
-      <c r="B18" s="25" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="51"/>
-      <c r="B19" s="25" t="s">
-        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -4356,47 +4408,47 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="42"/>
+      <c r="B2" s="44"/>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="7" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="42"/>
+      <c r="B7" s="44"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="11" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="42"/>
+      <c r="B11" s="44"/>
     </row>
     <row r="12" spans="1:2" ht="30">
       <c r="A12" s="19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="19" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>